<commit_message>
* Working on new powerdistribution method.
</commit_message>
<xml_diff>
--- a/doc/memmap.xlsx
+++ b/doc/memmap.xlsx
@@ -5,7 +5,7 @@
   <workbookPr defaultThemeVersion="153222"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\dmouse\ownCloud\Projects\KiCAD\stackable_z80_computer\doc\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\dmouse\ownCloud\Projects\KiCAD\SZC-1\doc\"/>
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
@@ -24,7 +24,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="87" uniqueCount="56">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="93" uniqueCount="57">
   <si>
     <t>SLOT0</t>
   </si>
@@ -155,18 +155,9 @@
     <t>MAPPER</t>
   </si>
   <si>
-    <t>#B8</t>
-  </si>
-  <si>
     <t>DIAG</t>
   </si>
   <si>
-    <t>Diagnostics card</t>
-  </si>
-  <si>
-    <t>RTC</t>
-  </si>
-  <si>
     <t>EXP-ROM</t>
   </si>
   <si>
@@ -179,19 +170,31 @@
     <t>GLOBAL MEMORY MAP (without the PPI board)</t>
   </si>
   <si>
-    <t>#B4-#B8</t>
-  </si>
-  <si>
     <t>Real Time Clock card</t>
   </si>
   <si>
-    <t>3 (but configurable as /INT, 1, 2, or 3)</t>
-  </si>
-  <si>
     <t>5 (but configurable as /INT, 4, 5, or 7)</t>
   </si>
   <si>
     <t>4 (but configurable as /INT, 4, 5, or 7)</t>
+  </si>
+  <si>
+    <t>#B4-#B7</t>
+  </si>
+  <si>
+    <t>#B8-#BF</t>
+  </si>
+  <si>
+    <t>Diagnostics card (does not decode A0-A2)</t>
+  </si>
+  <si>
+    <t>3 (but configurable as /NMI, /INT, 0, or 3)</t>
+  </si>
+  <si>
+    <t>PIT</t>
+  </si>
+  <si>
+    <t>3 (but configurable as /INT, 5, 6, or 7)</t>
   </si>
 </sst>
 </file>
@@ -530,10 +533,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:J35"/>
+  <dimension ref="A1:J36"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="A13" workbookViewId="0">
-      <selection activeCell="E30" sqref="E30"/>
+      <selection activeCell="E31" sqref="E31"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -541,13 +544,13 @@
     <col min="2" max="2" width="9.33203125" style="4" bestFit="1" customWidth="1"/>
     <col min="3" max="3" width="9.33203125" customWidth="1"/>
     <col min="4" max="4" width="19.6640625" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="31.5546875" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="35" bestFit="1" customWidth="1"/>
     <col min="6" max="6" width="18.109375" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A1" s="1" t="s">
-        <v>50</v>
+        <v>47</v>
       </c>
     </row>
     <row r="5" spans="1:9" x14ac:dyDescent="0.3">
@@ -615,7 +618,7 @@
     </row>
     <row r="11" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A11" s="1" t="s">
-        <v>49</v>
+        <v>46</v>
       </c>
     </row>
     <row r="13" spans="1:9" x14ac:dyDescent="0.3">
@@ -692,12 +695,12 @@
         <v>10</v>
       </c>
       <c r="B18" s="5" t="s">
-        <v>48</v>
+        <v>45</v>
       </c>
       <c r="C18" s="2"/>
       <c r="D18" s="2"/>
       <c r="E18" s="2" t="s">
-        <v>47</v>
+        <v>44</v>
       </c>
       <c r="F18" s="2"/>
       <c r="G18" s="2" t="s">
@@ -718,7 +721,7 @@
       <c r="C19" s="2"/>
       <c r="D19" s="2"/>
       <c r="E19" s="2" t="s">
-        <v>47</v>
+        <v>44</v>
       </c>
       <c r="F19" s="2"/>
       <c r="G19" s="2" t="s">
@@ -825,7 +828,7 @@
         <v>39</v>
       </c>
       <c r="E27" t="s">
-        <v>54</v>
+        <v>49</v>
       </c>
     </row>
     <row r="28" spans="1:10" x14ac:dyDescent="0.3">
@@ -842,7 +845,7 @@
         <v>41</v>
       </c>
       <c r="E28" t="s">
-        <v>55</v>
+        <v>50</v>
       </c>
     </row>
     <row r="29" spans="1:10" x14ac:dyDescent="0.3">
@@ -856,13 +859,13 @@
         <v>51</v>
       </c>
       <c r="D29" t="s">
-        <v>46</v>
+        <v>55</v>
       </c>
       <c r="E29" t="s">
-        <v>53</v>
+        <v>54</v>
       </c>
       <c r="F29" t="s">
-        <v>52</v>
+        <v>48</v>
       </c>
     </row>
     <row r="30" spans="1:10" x14ac:dyDescent="0.3">
@@ -873,20 +876,40 @@
         <v>32</v>
       </c>
       <c r="C30" t="s">
+        <v>51</v>
+      </c>
+      <c r="D30" t="s">
+        <v>55</v>
+      </c>
+      <c r="E30" t="s">
+        <v>56</v>
+      </c>
+      <c r="F30" t="s">
+        <v>48</v>
+      </c>
+    </row>
+    <row r="31" spans="1:10" x14ac:dyDescent="0.3">
+      <c r="A31" t="s">
+        <v>25</v>
+      </c>
+      <c r="B31" s="3" t="s">
+        <v>32</v>
+      </c>
+      <c r="C31" t="s">
+        <v>52</v>
+      </c>
+      <c r="D31" t="s">
         <v>43</v>
       </c>
-      <c r="D30" t="s">
-        <v>44</v>
-      </c>
-      <c r="E30" t="s">
+      <c r="E31" t="s">
         <v>37</v>
       </c>
-      <c r="F30" t="s">
-        <v>45</v>
-      </c>
-    </row>
-    <row r="35" spans="6:6" x14ac:dyDescent="0.3">
-      <c r="F35" t="s">
+      <c r="F31" t="s">
+        <v>53</v>
+      </c>
+    </row>
+    <row r="36" spans="6:6" x14ac:dyDescent="0.3">
+      <c r="F36" t="s">
         <v>38</v>
       </c>
     </row>

</xml_diff>

<commit_message>
Genera update of renderings and specifications
</commit_message>
<xml_diff>
--- a/doc/memmap.xlsx
+++ b/doc/memmap.xlsx
@@ -5,12 +5,13 @@
   <workbookPr backupFile="false" showObjects="all" date1904="false"/>
   <workbookProtection/>
   <bookViews>
-    <workbookView showHorizontalScroll="true" showVerticalScroll="true" showSheetTabs="true" xWindow="0" yWindow="0" windowWidth="16384" windowHeight="8192" tabRatio="500" firstSheet="0" activeTab="0"/>
+    <workbookView showHorizontalScroll="true" showVerticalScroll="true" showSheetTabs="true" xWindow="0" yWindow="0" windowWidth="16384" windowHeight="8192" tabRatio="500" firstSheet="0" activeTab="1"/>
   </bookViews>
   <sheets>
     <sheet name="Global IO Map" sheetId="1" state="visible" r:id="rId2"/>
     <sheet name="Global Memory Map" sheetId="2" state="visible" r:id="rId3"/>
     <sheet name="Global Slot Map" sheetId="3" state="visible" r:id="rId4"/>
+    <sheet name="MMU Schematic" sheetId="4" state="visible" r:id="rId5"/>
   </sheets>
   <calcPr iterateCount="100" refMode="A1" iterate="false" iterateDelta="0.0001"/>
   <extLst>
@@ -22,7 +23,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="164" uniqueCount="100">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="224" uniqueCount="138">
   <si>
     <t xml:space="preserve">GLOBAL I/O MAP</t>
   </si>
@@ -51,7 +52,7 @@
     <t xml:space="preserve">Expansion Connector B pin usage</t>
   </si>
   <si>
-    <t xml:space="preserve">Expansion Connector C usage</t>
+    <t xml:space="preserve">Expansion Connector C Pin usage</t>
   </si>
   <si>
     <t xml:space="preserve">MMIO</t>
@@ -60,7 +61,7 @@
     <t xml:space="preserve">0</t>
   </si>
   <si>
-    <t xml:space="preserve">#FFFFF</t>
+    <t xml:space="preserve">$FFFFF</t>
   </si>
   <si>
     <t xml:space="preserve">Secondary slot register</t>
@@ -84,7 +85,7 @@
     <t xml:space="preserve">#FC-#FF</t>
   </si>
   <si>
-    <t xml:space="preserve">MMU / PPI Slot select</t>
+    <t xml:space="preserve">MMU</t>
   </si>
   <si>
     <t xml:space="preserve">#F0-#F1</t>
@@ -141,13 +142,22 @@
     <t xml:space="preserve">PPI</t>
   </si>
   <si>
-    <t xml:space="preserve">#A0-#A7</t>
-  </si>
-  <si>
-    <t xml:space="preserve">PSG</t>
-  </si>
-  <si>
-    <t xml:space="preserve">PSG Audio Interface</t>
+    <t xml:space="preserve">#A4-#A7</t>
+  </si>
+  <si>
+    <t xml:space="preserve">PSG (secondary)</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Primary PSG Audio Interface</t>
+  </si>
+  <si>
+    <t xml:space="preserve">#A0-#A3</t>
+  </si>
+  <si>
+    <t xml:space="preserve">PSG (primary)</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Secondary PSG Audio Interface</t>
   </si>
   <si>
     <t xml:space="preserve">#90-#91</t>
@@ -228,7 +238,7 @@
     <t xml:space="preserve">SEGMENT #</t>
   </si>
   <si>
-    <t xml:space="preserve">VIRTUAL ADDRESS</t>
+    <t xml:space="preserve">PHYSICAL ADDRESS</t>
   </si>
   <si>
     <t xml:space="preserve">#FFFF</t>
@@ -286,6 +296,111 @@
   </si>
   <si>
     <t xml:space="preserve">#0000</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Segment 0 (the very first 16kB of the entire 4MB virtual address space) must always be ROM, as the MMU does not initialize the memory map on /RESET,</t>
+  </si>
+  <si>
+    <t xml:space="preserve">and it is to be assumed that all 8-bit page registers are set to 0, which means that after reset, that segment 0 is selected in all 4 16kB pages.</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Simple MMU diagram (complete schematic in the “MMU Schematic” worksheet):</t>
+  </si>
+  <si>
+    <t xml:space="preserve">CPU SIDE</t>
+  </si>
+  <si>
+    <t xml:space="preserve">MMU Input</t>
+  </si>
+  <si>
+    <t xml:space="preserve">MMU register</t>
+  </si>
+  <si>
+    <t xml:space="preserve">MMU output</t>
+  </si>
+  <si>
+    <t xml:space="preserve">BUS SIDE</t>
+  </si>
+  <si>
+    <t xml:space="preserve">A0..A13</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Bypassed</t>
+  </si>
+  <si>
+    <t xml:space="preserve">A14..A15</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Page register select</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Segment for page 0</t>
+  </si>
+  <si>
+    <t xml:space="preserve">A14..A21</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Segment for page 1</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Segment for page 2</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Segment for page 3</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Virtual address calculation example</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Z80 address</t>
+  </si>
+  <si>
+    <t xml:space="preserve">MMU register value</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Physical address</t>
+  </si>
+  <si>
+    <t xml:space="preserve">MMU Registers</t>
+  </si>
+  <si>
+    <t xml:space="preserve">MMU register values</t>
+  </si>
+  <si>
+    <t xml:space="preserve">#1000</t>
+  </si>
+  <si>
+    <t xml:space="preserve">#2000</t>
+  </si>
+  <si>
+    <t xml:space="preserve">#3000</t>
+  </si>
+  <si>
+    <t xml:space="preserve">#5000</t>
+  </si>
+  <si>
+    <t xml:space="preserve">#6000</t>
+  </si>
+  <si>
+    <t xml:space="preserve">#7000</t>
+  </si>
+  <si>
+    <t xml:space="preserve">#9000</t>
+  </si>
+  <si>
+    <t xml:space="preserve">#A000</t>
+  </si>
+  <si>
+    <t xml:space="preserve">#B000</t>
+  </si>
+  <si>
+    <t xml:space="preserve">#D000</t>
+  </si>
+  <si>
+    <t xml:space="preserve">#E000</t>
+  </si>
+  <si>
+    <t xml:space="preserve">#F000</t>
   </si>
   <si>
     <t xml:space="preserve">GLOBAL SLOT MAP (when using the PPI board)</t>
@@ -328,9 +443,11 @@
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
-  <numFmts count="2">
+  <numFmts count="4">
     <numFmt numFmtId="164" formatCode="General"/>
     <numFmt numFmtId="165" formatCode="@"/>
+    <numFmt numFmtId="166" formatCode="General"/>
+    <numFmt numFmtId="167" formatCode="[$$-409]#,##0.00;[RED]\-[$$-409]#,##0.00"/>
   </numFmts>
   <fonts count="5">
     <font>
@@ -412,7 +529,7 @@
     <xf numFmtId="42" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
     <xf numFmtId="9" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
   </cellStyleXfs>
-  <cellXfs count="9">
+  <cellXfs count="12">
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="false" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
@@ -442,6 +559,18 @@
       <protection locked="true" hidden="false"/>
     </xf>
     <xf numFmtId="164" fontId="0" fillId="2" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="false" applyProtection="false">
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="166" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="false" applyProtection="false">
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="false" applyProtection="false">
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="167" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
@@ -521,18 +650,60 @@
 </styleSheet>
 </file>
 
+<file path=xl/drawings/drawing1.xml><?xml version="1.0" encoding="utf-8"?>
+<xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+  <xdr:twoCellAnchor editAs="oneCell">
+    <xdr:from>
+      <xdr:col>1</xdr:col>
+      <xdr:colOff>0</xdr:colOff>
+      <xdr:row>1</xdr:row>
+      <xdr:rowOff>0</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>12</xdr:col>
+      <xdr:colOff>693360</xdr:colOff>
+      <xdr:row>34</xdr:row>
+      <xdr:rowOff>162360</xdr:rowOff>
+    </xdr:to>
+    <xdr:pic>
+      <xdr:nvPicPr>
+        <xdr:cNvPr id="0" name="Image 1" descr=""/>
+        <xdr:cNvPicPr/>
+      </xdr:nvPicPr>
+      <xdr:blipFill>
+        <a:blip r:embed="rId1"/>
+        <a:stretch/>
+      </xdr:blipFill>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="812520" y="162360"/>
+          <a:ext cx="9634320" cy="5526720"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+        <a:ln w="0">
+          <a:noFill/>
+        </a:ln>
+      </xdr:spPr>
+    </xdr:pic>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+</xdr:wsDr>
+</file>
+
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
   <sheetPr filterMode="false">
     <pageSetUpPr fitToPage="false"/>
   </sheetPr>
-  <dimension ref="A2:I20"/>
+  <dimension ref="A2:I1048576"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="C9" activeCellId="0" sqref="C9"/>
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="140" zoomScaleNormal="140" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="D11" activeCellId="0" sqref="D11"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="8.72265625" defaultRowHeight="14.4" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="8.75" defaultRowHeight="14.4" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="0" width="16.11"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="1" width="7.44"/>
@@ -541,7 +712,7 @@
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="6" min="5" style="0" width="40"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="7" min="7" style="0" width="39.55"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="8" min="8" style="0" width="30.66"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="9" min="9" style="0" width="27.33"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="9" min="9" style="0" width="29.77"/>
   </cols>
   <sheetData>
     <row r="2" customFormat="false" ht="14.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -750,7 +921,7 @@
       </c>
       <c r="G11" s="6"/>
     </row>
-    <row r="12" customFormat="false" ht="14.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="12" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A12" s="0" t="s">
         <v>17</v>
       </c>
@@ -772,8 +943,14 @@
       <c r="G12" s="6" t="s">
         <v>41</v>
       </c>
-    </row>
-    <row r="13" customFormat="false" ht="14.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="H12" s="0" t="s">
+        <v>14</v>
+      </c>
+      <c r="I12" s="0" t="s">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="13" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A13" s="0" t="s">
         <v>17</v>
       </c>
@@ -787,13 +964,19 @@
         <v>43</v>
       </c>
       <c r="E13" s="0" t="s">
+        <v>14</v>
+      </c>
+      <c r="F13" s="0" t="s">
+        <v>14</v>
+      </c>
+      <c r="G13" s="6" t="s">
         <v>44</v>
       </c>
-      <c r="F13" s="0" t="s">
-        <v>14</v>
-      </c>
-      <c r="G13" s="6" t="s">
-        <v>45</v>
+      <c r="H13" s="0" t="s">
+        <v>14</v>
+      </c>
+      <c r="I13" s="0" t="s">
+        <v>14</v>
       </c>
     </row>
     <row r="14" customFormat="false" ht="14.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -804,18 +987,20 @@
         <v>18</v>
       </c>
       <c r="C14" s="0" t="s">
+        <v>45</v>
+      </c>
+      <c r="D14" s="0" t="s">
         <v>46</v>
       </c>
-      <c r="D14" s="0" t="s">
+      <c r="E14" s="0" t="s">
         <v>47</v>
       </c>
-      <c r="E14" s="0" t="s">
+      <c r="F14" s="0" t="s">
+        <v>14</v>
+      </c>
+      <c r="G14" s="6" t="s">
         <v>48</v>
       </c>
-      <c r="F14" s="0" t="s">
-        <v>14</v>
-      </c>
-      <c r="G14" s="6"/>
     </row>
     <row r="15" customFormat="false" ht="14.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A15" s="0" t="s">
@@ -855,25 +1040,47 @@
         <v>54</v>
       </c>
       <c r="F16" s="0" t="s">
+        <v>14</v>
+      </c>
+      <c r="G16" s="6"/>
+    </row>
+    <row r="17" customFormat="false" ht="14.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A17" s="0" t="s">
+        <v>17</v>
+      </c>
+      <c r="B17" s="5" t="s">
+        <v>18</v>
+      </c>
+      <c r="C17" s="0" t="s">
         <v>55</v>
       </c>
-      <c r="G16" s="6" t="s">
+      <c r="D17" s="0" t="s">
         <v>56</v>
       </c>
-    </row>
-    <row r="18" customFormat="false" ht="14.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A18" s="0" t="s">
+      <c r="E17" s="0" t="s">
         <v>57</v>
       </c>
-      <c r="B18" s="1" t="s">
+      <c r="F17" s="0" t="s">
         <v>58</v>
       </c>
-    </row>
-    <row r="20" customFormat="false" ht="14.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="G20" s="0" t="s">
+      <c r="G17" s="6" t="s">
         <v>59</v>
       </c>
     </row>
+    <row r="19" customFormat="false" ht="14.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A19" s="0" t="s">
+        <v>60</v>
+      </c>
+      <c r="B19" s="1" t="s">
+        <v>61</v>
+      </c>
+    </row>
+    <row r="21" customFormat="false" ht="14.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="G21" s="0" t="s">
+        <v>62</v>
+      </c>
+    </row>
+    <row r="1048576" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
   </sheetData>
   <printOptions headings="false" gridLines="false" gridLinesSet="true" horizontalCentered="false" verticalCentered="false"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.511805555555555" footer="0.511805555555555"/>
@@ -890,38 +1097,41 @@
   <sheetPr filterMode="false">
     <pageSetUpPr fitToPage="false"/>
   </sheetPr>
-  <dimension ref="A1:O10"/>
+  <dimension ref="A1:O42"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="M4" activeCellId="0" sqref="M4"/>
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A9" colorId="64" zoomScale="140" zoomScaleNormal="140" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="A43" activeCellId="0" sqref="A43"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="8.72265625" defaultRowHeight="14.4" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="8.75" defaultRowHeight="14.4" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="0" width="8.44"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="4" min="4" style="0" width="6.11"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="8" min="8" style="0" width="10.58"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="9" min="9" style="0" width="26"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="10" min="10" style="0" width="16.67"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="14" min="14" style="0" width="26"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="15" min="15" style="0" width="16.67"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="0" width="11.52"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="0" width="17.59"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="3" min="3" style="0" width="17.88"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="4" min="4" style="0" width="12.63"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="5" min="5" style="0" width="15.31"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="8" min="8" style="0" width="17.36"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="9" min="9" style="0" width="26.58"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="10" min="10" style="0" width="16.99"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="14" min="13" style="0" width="26.58"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="15" min="15" style="0" width="16.99"/>
   </cols>
   <sheetData>
     <row r="1" customFormat="false" ht="14.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A1" s="2" t="s">
-        <v>60</v>
+        <v>63</v>
       </c>
       <c r="H1" s="2" t="s">
-        <v>61</v>
+        <v>64</v>
       </c>
     </row>
     <row r="2" customFormat="false" ht="14.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A2" s="2" t="s">
-        <v>62</v>
+        <v>65</v>
       </c>
       <c r="B2" s="1"/>
       <c r="H2" s="2" t="s">
-        <v>63</v>
+        <v>66</v>
       </c>
     </row>
     <row r="3" customFormat="false" ht="14.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -930,15 +1140,15 @@
     <row r="4" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B4" s="1"/>
       <c r="H4" s="2" t="s">
-        <v>64</v>
+        <v>67</v>
       </c>
       <c r="M4" s="2" t="s">
-        <v>65</v>
+        <v>68</v>
       </c>
     </row>
     <row r="5" customFormat="false" ht="14.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A5" s="2" t="s">
-        <v>66</v>
+        <v>69</v>
       </c>
       <c r="B5" s="2" t="s">
         <v>4</v>
@@ -948,113 +1158,596 @@
         <v>3</v>
       </c>
       <c r="H5" s="2" t="s">
-        <v>67</v>
+        <v>70</v>
       </c>
       <c r="I5" s="2" t="s">
         <v>4</v>
       </c>
       <c r="J5" s="2" t="s">
-        <v>68</v>
+        <v>71</v>
       </c>
       <c r="M5" s="2" t="s">
-        <v>67</v>
+        <v>70</v>
       </c>
       <c r="N5" s="2" t="s">
         <v>4</v>
       </c>
       <c r="O5" s="2" t="s">
-        <v>68</v>
+        <v>71</v>
       </c>
     </row>
     <row r="6" customFormat="false" ht="14.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B6" s="7"/>
       <c r="C6" s="7"/>
       <c r="D6" s="0" t="s">
-        <v>69</v>
+        <v>72</v>
       </c>
       <c r="H6" s="0" t="s">
-        <v>70</v>
+        <v>73</v>
       </c>
       <c r="I6" s="7" t="s">
-        <v>71</v>
+        <v>74</v>
       </c>
       <c r="J6" s="0" t="s">
-        <v>72</v>
+        <v>75</v>
       </c>
       <c r="M6" s="0" t="s">
-        <v>73</v>
+        <v>76</v>
       </c>
       <c r="N6" s="7" t="s">
-        <v>71</v>
+        <v>74</v>
       </c>
       <c r="O6" s="0" t="s">
-        <v>72</v>
+        <v>75</v>
       </c>
     </row>
     <row r="7" customFormat="false" ht="14.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A7" s="0" t="s">
-        <v>74</v>
+        <v>77</v>
       </c>
       <c r="B7" s="7" t="s">
-        <v>75</v>
+        <v>78</v>
       </c>
       <c r="C7" s="7"/>
       <c r="D7" s="0" t="s">
-        <v>76</v>
+        <v>79</v>
       </c>
       <c r="H7" s="0" t="s">
-        <v>77</v>
+        <v>80</v>
       </c>
       <c r="I7" s="7" t="s">
-        <v>78</v>
+        <v>81</v>
       </c>
       <c r="J7" s="0" t="s">
-        <v>79</v>
+        <v>82</v>
       </c>
       <c r="M7" s="0" t="s">
-        <v>80</v>
+        <v>83</v>
       </c>
       <c r="N7" s="7" t="s">
-        <v>78</v>
+        <v>81</v>
       </c>
       <c r="O7" s="0" t="s">
-        <v>81</v>
+        <v>84</v>
       </c>
     </row>
     <row r="8" customFormat="false" ht="14.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A8" s="0" t="s">
-        <v>82</v>
+        <v>85</v>
       </c>
       <c r="B8" s="7" t="s">
-        <v>75</v>
+        <v>78</v>
       </c>
       <c r="C8" s="7"/>
       <c r="D8" s="0" t="s">
-        <v>83</v>
+        <v>86</v>
       </c>
     </row>
     <row r="9" customFormat="false" ht="14.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A9" s="0" t="s">
-        <v>84</v>
+        <v>87</v>
       </c>
       <c r="B9" s="7" t="s">
-        <v>75</v>
+        <v>78</v>
       </c>
       <c r="C9" s="7"/>
       <c r="D9" s="0" t="s">
-        <v>85</v>
+        <v>88</v>
       </c>
     </row>
     <row r="10" customFormat="false" ht="14.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A10" s="0" t="s">
-        <v>86</v>
+        <v>89</v>
       </c>
       <c r="B10" s="7" t="s">
-        <v>75</v>
+        <v>78</v>
       </c>
       <c r="C10" s="7"/>
       <c r="D10" s="0" t="s">
-        <v>87</v>
+        <v>90</v>
+      </c>
+    </row>
+    <row r="12" customFormat="false" ht="14.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A12" s="0" t="s">
+        <v>91</v>
+      </c>
+    </row>
+    <row r="13" customFormat="false" ht="14.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A13" s="0" t="s">
+        <v>92</v>
+      </c>
+    </row>
+    <row r="15" customFormat="false" ht="14.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A15" s="0" t="s">
+        <v>93</v>
+      </c>
+    </row>
+    <row r="16" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
+    <row r="17" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A17" s="2" t="s">
+        <v>94</v>
+      </c>
+      <c r="B17" s="2" t="s">
+        <v>95</v>
+      </c>
+      <c r="C17" s="2" t="s">
+        <v>96</v>
+      </c>
+      <c r="D17" s="2" t="s">
+        <v>97</v>
+      </c>
+      <c r="E17" s="2" t="s">
+        <v>98</v>
+      </c>
+    </row>
+    <row r="18" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A18" s="0" t="s">
+        <v>99</v>
+      </c>
+      <c r="C18" s="0" t="s">
+        <v>100</v>
+      </c>
+      <c r="E18" s="0" t="s">
+        <v>99</v>
+      </c>
+    </row>
+    <row r="19" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A19" s="0" t="s">
+        <v>101</v>
+      </c>
+      <c r="B19" s="0" t="s">
+        <v>102</v>
+      </c>
+      <c r="C19" s="0" t="s">
+        <v>103</v>
+      </c>
+      <c r="D19" s="0" t="s">
+        <v>104</v>
+      </c>
+      <c r="E19" s="0" t="s">
+        <v>104</v>
+      </c>
+    </row>
+    <row r="20" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="C20" s="0" t="s">
+        <v>105</v>
+      </c>
+      <c r="D20" s="0" t="s">
+        <v>104</v>
+      </c>
+      <c r="E20" s="0" t="s">
+        <v>104</v>
+      </c>
+    </row>
+    <row r="21" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="C21" s="0" t="s">
+        <v>106</v>
+      </c>
+      <c r="D21" s="0" t="s">
+        <v>104</v>
+      </c>
+      <c r="E21" s="0" t="s">
+        <v>104</v>
+      </c>
+    </row>
+    <row r="22" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="C22" s="0" t="s">
+        <v>107</v>
+      </c>
+      <c r="D22" s="0" t="s">
+        <v>104</v>
+      </c>
+      <c r="E22" s="0" t="s">
+        <v>104</v>
+      </c>
+    </row>
+    <row r="24" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A24" s="2" t="s">
+        <v>108</v>
+      </c>
+    </row>
+    <row r="25" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
+    <row r="26" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A26" s="2" t="s">
+        <v>109</v>
+      </c>
+      <c r="B26" s="2" t="s">
+        <v>95</v>
+      </c>
+      <c r="C26" s="2" t="s">
+        <v>110</v>
+      </c>
+      <c r="D26" s="2" t="s">
+        <v>97</v>
+      </c>
+      <c r="E26" s="2" t="s">
+        <v>111</v>
+      </c>
+      <c r="H26" s="2" t="s">
+        <v>112</v>
+      </c>
+      <c r="I26" s="2" t="s">
+        <v>113</v>
+      </c>
+    </row>
+    <row r="27" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A27" s="0" t="s">
+        <v>90</v>
+      </c>
+      <c r="B27" s="0" t="n">
+        <f aca="false">_xlfn.BITRSHIFT(HEX2DEC(MID($A27, 2, LEN($A27))), 14)</f>
+        <v>0</v>
+      </c>
+      <c r="C27" s="0" t="n">
+        <f aca="false">VLOOKUP($B27,$H$27:$I30, 2, 0)</f>
+        <v>0</v>
+      </c>
+      <c r="D27" s="8" t="str">
+        <f aca="false">DEC2HEX($C27, 2)</f>
+        <v>00</v>
+      </c>
+      <c r="E27" s="9" t="str">
+        <f aca="false">_xlfn.CONCAT("#", DEC2HEX(_xlfn.BITOR(_xlfn.BITLSHIFT($C27, 14), _xlfn.BITAND(HEX2DEC(MID($A27, 2, LEN($A27))), 16383)), 6))</f>
+        <v>#000000</v>
+      </c>
+      <c r="H27" s="0" t="n">
+        <v>0</v>
+      </c>
+      <c r="I27" s="0" t="n">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="28" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A28" s="0" t="s">
+        <v>114</v>
+      </c>
+      <c r="B28" s="0" t="n">
+        <f aca="false">_xlfn.BITRSHIFT(HEX2DEC(MID($A28, 2, LEN($A28))), 14)</f>
+        <v>0</v>
+      </c>
+      <c r="C28" s="0" t="n">
+        <f aca="false">VLOOKUP($B28,$H$27:$I31, 2, 0)</f>
+        <v>0</v>
+      </c>
+      <c r="D28" s="8" t="str">
+        <f aca="false">DEC2HEX($C28, 2)</f>
+        <v>00</v>
+      </c>
+      <c r="E28" s="9" t="str">
+        <f aca="false">_xlfn.CONCAT("#", DEC2HEX(_xlfn.BITOR(_xlfn.BITLSHIFT($C28, 14), _xlfn.BITAND(HEX2DEC(MID($A28, 2, LEN($A28))), 16383)), 6))</f>
+        <v>#001000</v>
+      </c>
+      <c r="H28" s="0" t="n">
+        <v>1</v>
+      </c>
+      <c r="I28" s="0" t="n">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="29" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A29" s="10" t="s">
+        <v>115</v>
+      </c>
+      <c r="B29" s="0" t="n">
+        <f aca="false">_xlfn.BITRSHIFT(HEX2DEC(MID($A29, 2, LEN($A29))), 14)</f>
+        <v>0</v>
+      </c>
+      <c r="C29" s="0" t="n">
+        <f aca="false">VLOOKUP($B29,$H$27:$I32, 2, 0)</f>
+        <v>0</v>
+      </c>
+      <c r="D29" s="8" t="str">
+        <f aca="false">DEC2HEX($C29, 2)</f>
+        <v>00</v>
+      </c>
+      <c r="E29" s="9" t="str">
+        <f aca="false">_xlfn.CONCAT("#", DEC2HEX(_xlfn.BITOR(_xlfn.BITLSHIFT($C29, 14), _xlfn.BITAND(HEX2DEC(MID($A29, 2, LEN($A29))), 16383)), 6))</f>
+        <v>#002000</v>
+      </c>
+      <c r="H29" s="0" t="n">
+        <v>2</v>
+      </c>
+      <c r="I29" s="0" t="n">
+        <v>126</v>
+      </c>
+    </row>
+    <row r="30" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A30" s="0" t="s">
+        <v>116</v>
+      </c>
+      <c r="B30" s="0" t="n">
+        <f aca="false">_xlfn.BITRSHIFT(HEX2DEC(MID($A30, 2, LEN($A30))), 14)</f>
+        <v>0</v>
+      </c>
+      <c r="C30" s="0" t="n">
+        <f aca="false">VLOOKUP($B30,$H$27:$I33, 2, 0)</f>
+        <v>0</v>
+      </c>
+      <c r="D30" s="8" t="str">
+        <f aca="false">DEC2HEX($C30, 2)</f>
+        <v>00</v>
+      </c>
+      <c r="E30" s="9" t="str">
+        <f aca="false">_xlfn.CONCAT("#", DEC2HEX(_xlfn.BITOR(_xlfn.BITLSHIFT($C30, 14), _xlfn.BITAND(HEX2DEC(MID($A30, 2, LEN($A30))), 16383)), 6))</f>
+        <v>#003000</v>
+      </c>
+      <c r="H30" s="0" t="n">
+        <v>3</v>
+      </c>
+      <c r="I30" s="0" t="n">
+        <v>127</v>
+      </c>
+    </row>
+    <row r="31" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A31" s="0" t="s">
+        <v>88</v>
+      </c>
+      <c r="B31" s="0" t="n">
+        <f aca="false">_xlfn.BITRSHIFT(HEX2DEC(MID($A31, 2, LEN($A31))), 14)</f>
+        <v>1</v>
+      </c>
+      <c r="C31" s="0" t="n">
+        <f aca="false">VLOOKUP($B31,$H$27:$I34, 2, 0)</f>
+        <v>1</v>
+      </c>
+      <c r="D31" s="8" t="str">
+        <f aca="false">DEC2HEX($C31, 2)</f>
+        <v>01</v>
+      </c>
+      <c r="E31" s="9" t="str">
+        <f aca="false">_xlfn.CONCAT("#", DEC2HEX(_xlfn.BITOR(_xlfn.BITLSHIFT($C31, 14), _xlfn.BITAND(HEX2DEC(MID($A31, 2, LEN($A31))), 16383)), 6))</f>
+        <v>#004000</v>
+      </c>
+    </row>
+    <row r="32" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A32" s="0" t="s">
+        <v>117</v>
+      </c>
+      <c r="B32" s="0" t="n">
+        <f aca="false">_xlfn.BITRSHIFT(HEX2DEC(MID($A32, 2, LEN($A32))), 14)</f>
+        <v>1</v>
+      </c>
+      <c r="C32" s="0" t="n">
+        <f aca="false">VLOOKUP($B32,$H$27:$I35, 2, 0)</f>
+        <v>1</v>
+      </c>
+      <c r="D32" s="8" t="str">
+        <f aca="false">DEC2HEX($C32, 2)</f>
+        <v>01</v>
+      </c>
+      <c r="E32" s="9" t="str">
+        <f aca="false">_xlfn.CONCAT("#", DEC2HEX(_xlfn.BITOR(_xlfn.BITLSHIFT($C32, 14), _xlfn.BITAND(HEX2DEC(MID($A32, 2, LEN($A32))), 16383)), 6))</f>
+        <v>#005000</v>
+      </c>
+    </row>
+    <row r="33" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A33" s="0" t="s">
+        <v>118</v>
+      </c>
+      <c r="B33" s="0" t="n">
+        <f aca="false">_xlfn.BITRSHIFT(HEX2DEC(MID($A33, 2, LEN($A33))), 14)</f>
+        <v>1</v>
+      </c>
+      <c r="C33" s="0" t="n">
+        <f aca="false">VLOOKUP($B33,$H$27:$I36, 2, 0)</f>
+        <v>1</v>
+      </c>
+      <c r="D33" s="8" t="str">
+        <f aca="false">DEC2HEX($C33, 2)</f>
+        <v>01</v>
+      </c>
+      <c r="E33" s="9" t="str">
+        <f aca="false">_xlfn.CONCAT("#", DEC2HEX(_xlfn.BITOR(_xlfn.BITLSHIFT($C33, 14), _xlfn.BITAND(HEX2DEC(MID($A33, 2, LEN($A33))), 16383)), 6))</f>
+        <v>#006000</v>
+      </c>
+    </row>
+    <row r="34" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A34" s="0" t="s">
+        <v>119</v>
+      </c>
+      <c r="B34" s="0" t="n">
+        <f aca="false">_xlfn.BITRSHIFT(HEX2DEC(MID($A34, 2, LEN($A34))), 14)</f>
+        <v>1</v>
+      </c>
+      <c r="C34" s="0" t="n">
+        <f aca="false">VLOOKUP($B34,$H$27:$I37, 2, 0)</f>
+        <v>1</v>
+      </c>
+      <c r="D34" s="8" t="str">
+        <f aca="false">DEC2HEX($C34, 2)</f>
+        <v>01</v>
+      </c>
+      <c r="E34" s="9" t="str">
+        <f aca="false">_xlfn.CONCAT("#", DEC2HEX(_xlfn.BITOR(_xlfn.BITLSHIFT($C34, 14), _xlfn.BITAND(HEX2DEC(MID($A34, 2, LEN($A34))), 16383)), 6))</f>
+        <v>#007000</v>
+      </c>
+    </row>
+    <row r="35" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A35" s="0" t="s">
+        <v>86</v>
+      </c>
+      <c r="B35" s="0" t="n">
+        <f aca="false">_xlfn.BITRSHIFT(HEX2DEC(MID($A35, 2, LEN($A35))), 14)</f>
+        <v>2</v>
+      </c>
+      <c r="C35" s="0" t="n">
+        <f aca="false">VLOOKUP($B35,$H$27:$I38, 2, 0)</f>
+        <v>126</v>
+      </c>
+      <c r="D35" s="8" t="str">
+        <f aca="false">DEC2HEX($C35, 2)</f>
+        <v>7E</v>
+      </c>
+      <c r="E35" s="9" t="str">
+        <f aca="false">_xlfn.CONCAT("#", DEC2HEX(_xlfn.BITOR(_xlfn.BITLSHIFT($C35, 14), _xlfn.BITAND(HEX2DEC(MID($A35, 2, LEN($A35))), 16383)), 6))</f>
+        <v>#1F8000</v>
+      </c>
+    </row>
+    <row r="36" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A36" s="0" t="s">
+        <v>120</v>
+      </c>
+      <c r="B36" s="0" t="n">
+        <f aca="false">_xlfn.BITRSHIFT(HEX2DEC(MID($A36, 2, LEN($A36))), 14)</f>
+        <v>2</v>
+      </c>
+      <c r="C36" s="0" t="n">
+        <f aca="false">VLOOKUP($B36,$H$27:$I39, 2, 0)</f>
+        <v>126</v>
+      </c>
+      <c r="D36" s="8" t="str">
+        <f aca="false">DEC2HEX($C36, 2)</f>
+        <v>7E</v>
+      </c>
+      <c r="E36" s="9" t="str">
+        <f aca="false">_xlfn.CONCAT("#", DEC2HEX(_xlfn.BITOR(_xlfn.BITLSHIFT($C36, 14), _xlfn.BITAND(HEX2DEC(MID($A36, 2, LEN($A36))), 16383)), 6))</f>
+        <v>#1F9000</v>
+      </c>
+    </row>
+    <row r="37" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A37" s="10" t="s">
+        <v>121</v>
+      </c>
+      <c r="B37" s="0" t="n">
+        <f aca="false">_xlfn.BITRSHIFT(HEX2DEC(MID($A37, 2, LEN($A37))), 14)</f>
+        <v>2</v>
+      </c>
+      <c r="C37" s="0" t="n">
+        <f aca="false">VLOOKUP($B37,$H$27:$I40, 2, 0)</f>
+        <v>126</v>
+      </c>
+      <c r="D37" s="8" t="str">
+        <f aca="false">DEC2HEX($C37, 2)</f>
+        <v>7E</v>
+      </c>
+      <c r="E37" s="9" t="str">
+        <f aca="false">_xlfn.CONCAT("#", DEC2HEX(_xlfn.BITOR(_xlfn.BITLSHIFT($C37, 14), _xlfn.BITAND(HEX2DEC(MID($A37, 2, LEN($A37))), 16383)), 6))</f>
+        <v>#1FA000</v>
+      </c>
+    </row>
+    <row r="38" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A38" s="0" t="s">
+        <v>122</v>
+      </c>
+      <c r="B38" s="0" t="n">
+        <f aca="false">_xlfn.BITRSHIFT(HEX2DEC(MID($A38, 2, LEN($A38))), 14)</f>
+        <v>2</v>
+      </c>
+      <c r="C38" s="0" t="n">
+        <f aca="false">VLOOKUP($B38,$H$27:$I41, 2, 0)</f>
+        <v>126</v>
+      </c>
+      <c r="D38" s="8" t="str">
+        <f aca="false">DEC2HEX($C38, 2)</f>
+        <v>7E</v>
+      </c>
+      <c r="E38" s="9" t="str">
+        <f aca="false">_xlfn.CONCAT("#", DEC2HEX(_xlfn.BITOR(_xlfn.BITLSHIFT($C38, 14), _xlfn.BITAND(HEX2DEC(MID($A38, 2, LEN($A38))), 16383)), 6))</f>
+        <v>#1FB000</v>
+      </c>
+    </row>
+    <row r="39" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A39" s="0" t="s">
+        <v>79</v>
+      </c>
+      <c r="B39" s="0" t="n">
+        <f aca="false">_xlfn.BITRSHIFT(HEX2DEC(MID($A39, 2, LEN($A39))), 14)</f>
+        <v>3</v>
+      </c>
+      <c r="C39" s="0" t="n">
+        <f aca="false">VLOOKUP($B39,$H$27:$I42, 2, 0)</f>
+        <v>127</v>
+      </c>
+      <c r="D39" s="8" t="str">
+        <f aca="false">DEC2HEX($C39, 2)</f>
+        <v>7F</v>
+      </c>
+      <c r="E39" s="9" t="str">
+        <f aca="false">_xlfn.CONCAT("#", DEC2HEX(_xlfn.BITOR(_xlfn.BITLSHIFT($C39, 14), _xlfn.BITAND(HEX2DEC(MID($A39, 2, LEN($A39))), 16383)), 6))</f>
+        <v>#1FC000</v>
+      </c>
+    </row>
+    <row r="40" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A40" s="0" t="s">
+        <v>123</v>
+      </c>
+      <c r="B40" s="0" t="n">
+        <f aca="false">_xlfn.BITRSHIFT(HEX2DEC(MID($A40, 2, LEN($A40))), 14)</f>
+        <v>3</v>
+      </c>
+      <c r="C40" s="0" t="n">
+        <f aca="false">VLOOKUP($B40,$H$27:$I43, 2, 0)</f>
+        <v>127</v>
+      </c>
+      <c r="D40" s="8" t="str">
+        <f aca="false">DEC2HEX($C40, 2)</f>
+        <v>7F</v>
+      </c>
+      <c r="E40" s="9" t="str">
+        <f aca="false">_xlfn.CONCAT("#", DEC2HEX(_xlfn.BITOR(_xlfn.BITLSHIFT($C40, 14), _xlfn.BITAND(HEX2DEC(MID($A40, 2, LEN($A40))), 16383)), 6))</f>
+        <v>#1FD000</v>
+      </c>
+    </row>
+    <row r="41" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A41" s="0" t="s">
+        <v>124</v>
+      </c>
+      <c r="B41" s="0" t="n">
+        <f aca="false">_xlfn.BITRSHIFT(HEX2DEC(MID($A41, 2, LEN($A41))), 14)</f>
+        <v>3</v>
+      </c>
+      <c r="C41" s="0" t="n">
+        <f aca="false">VLOOKUP($B41,$H$27:$I44, 2, 0)</f>
+        <v>127</v>
+      </c>
+      <c r="D41" s="8" t="str">
+        <f aca="false">DEC2HEX($C41, 2)</f>
+        <v>7F</v>
+      </c>
+      <c r="E41" s="9" t="str">
+        <f aca="false">_xlfn.CONCAT("#", DEC2HEX(_xlfn.BITOR(_xlfn.BITLSHIFT($C41, 14), _xlfn.BITAND(HEX2DEC(MID($A41, 2, LEN($A41))), 16383)), 6))</f>
+        <v>#1FE000</v>
+      </c>
+    </row>
+    <row r="42" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A42" s="0" t="s">
+        <v>125</v>
+      </c>
+      <c r="B42" s="0" t="n">
+        <f aca="false">_xlfn.BITRSHIFT(HEX2DEC(MID($A42, 2, LEN($A42))), 14)</f>
+        <v>3</v>
+      </c>
+      <c r="C42" s="0" t="n">
+        <f aca="false">VLOOKUP($B42,$H$27:$I45, 2, 0)</f>
+        <v>127</v>
+      </c>
+      <c r="D42" s="8" t="str">
+        <f aca="false">DEC2HEX($C42, 2)</f>
+        <v>7F</v>
+      </c>
+      <c r="E42" s="9" t="str">
+        <f aca="false">_xlfn.CONCAT("#", DEC2HEX(_xlfn.BITOR(_xlfn.BITLSHIFT($C42, 14), _xlfn.BITAND(HEX2DEC(MID($A42, 2, LEN($A42))), 16383)), 6))</f>
+        <v>#1FF000</v>
       </c>
     </row>
   </sheetData>
@@ -1075,11 +1768,11 @@
   </sheetPr>
   <dimension ref="A2:J11"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="140" zoomScaleNormal="140" zoomScalePageLayoutView="100" workbookViewId="0">
       <selection pane="topLeft" activeCell="B4" activeCellId="0" sqref="B4"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="8.72265625" defaultRowHeight="14.4" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="8.75" defaultRowHeight="14.4" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="0" width="8.33"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="0" width="9.89"/>
@@ -1094,7 +1787,7 @@
   <sheetData>
     <row r="2" customFormat="false" ht="14.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A2" s="2" t="s">
-        <v>88</v>
+        <v>126</v>
       </c>
       <c r="B2" s="1"/>
     </row>
@@ -1103,32 +1796,32 @@
     </row>
     <row r="4" customFormat="false" ht="14.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B4" s="1" t="s">
-        <v>89</v>
+        <v>127</v>
       </c>
       <c r="C4" s="0" t="s">
-        <v>90</v>
+        <v>128</v>
       </c>
       <c r="D4" s="0" t="s">
-        <v>91</v>
+        <v>129</v>
       </c>
       <c r="E4" s="0" t="s">
-        <v>92</v>
+        <v>130</v>
       </c>
       <c r="F4" s="0" t="s">
-        <v>93</v>
+        <v>131</v>
       </c>
       <c r="G4" s="0" t="s">
-        <v>94</v>
+        <v>132</v>
       </c>
       <c r="H4" s="0" t="s">
-        <v>95</v>
+        <v>133</v>
       </c>
     </row>
     <row r="5" customFormat="false" ht="14.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B5" s="1"/>
     </row>
     <row r="6" customFormat="false" ht="14.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B6" s="8"/>
+      <c r="B6" s="11"/>
       <c r="C6" s="7"/>
       <c r="D6" s="7"/>
       <c r="E6" s="7"/>
@@ -1136,86 +1829,86 @@
       <c r="G6" s="7"/>
       <c r="H6" s="7"/>
       <c r="I6" s="0" t="s">
-        <v>69</v>
+        <v>72</v>
       </c>
     </row>
     <row r="7" customFormat="false" ht="14.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A7" s="0" t="s">
-        <v>74</v>
-      </c>
-      <c r="B7" s="8"/>
+        <v>77</v>
+      </c>
+      <c r="B7" s="11"/>
       <c r="C7" s="7"/>
       <c r="D7" s="7"/>
       <c r="E7" s="7"/>
       <c r="F7" s="7"/>
       <c r="G7" s="7" t="s">
-        <v>75</v>
+        <v>78</v>
       </c>
       <c r="H7" s="7"/>
       <c r="I7" s="0" t="s">
-        <v>76</v>
+        <v>79</v>
       </c>
     </row>
     <row r="8" customFormat="false" ht="14.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A8" s="0" t="s">
-        <v>82</v>
-      </c>
-      <c r="B8" s="8"/>
+        <v>85</v>
+      </c>
+      <c r="B8" s="11"/>
       <c r="C8" s="7"/>
       <c r="D8" s="7"/>
       <c r="E8" s="7"/>
       <c r="F8" s="7"/>
       <c r="G8" s="7" t="s">
-        <v>75</v>
+        <v>78</v>
       </c>
       <c r="H8" s="7"/>
       <c r="I8" s="0" t="s">
-        <v>83</v>
+        <v>86</v>
       </c>
     </row>
     <row r="9" customFormat="false" ht="14.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A9" s="0" t="s">
-        <v>84</v>
-      </c>
-      <c r="B9" s="8" t="s">
-        <v>96</v>
+        <v>87</v>
+      </c>
+      <c r="B9" s="11" t="s">
+        <v>134</v>
       </c>
       <c r="C9" s="7"/>
       <c r="D9" s="7"/>
       <c r="E9" s="7" t="s">
-        <v>97</v>
+        <v>135</v>
       </c>
       <c r="F9" s="7"/>
       <c r="G9" s="7" t="s">
-        <v>75</v>
+        <v>78</v>
       </c>
       <c r="H9" s="7"/>
       <c r="I9" s="0" t="s">
-        <v>85</v>
+        <v>88</v>
       </c>
     </row>
     <row r="10" customFormat="false" ht="14.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A10" s="0" t="s">
-        <v>86</v>
-      </c>
-      <c r="B10" s="8" t="s">
-        <v>98</v>
+        <v>89</v>
+      </c>
+      <c r="B10" s="11" t="s">
+        <v>136</v>
       </c>
       <c r="C10" s="7"/>
       <c r="D10" s="7"/>
       <c r="E10" s="7" t="s">
-        <v>97</v>
+        <v>135</v>
       </c>
       <c r="F10" s="7"/>
       <c r="G10" s="7" t="s">
-        <v>75</v>
+        <v>78</v>
       </c>
       <c r="H10" s="7"/>
       <c r="I10" s="0" t="s">
-        <v>87</v>
+        <v>90</v>
       </c>
       <c r="J10" s="0" t="s">
-        <v>99</v>
+        <v>137</v>
       </c>
     </row>
     <row r="11" customFormat="false" ht="14.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -1230,4 +1923,28 @@
     <oddFooter/>
   </headerFooter>
 </worksheet>
+</file>
+
+<file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+  <sheetPr filterMode="false">
+    <pageSetUpPr fitToPage="false"/>
+  </sheetPr>
+  <dimension ref="A1"/>
+  <sheetViews>
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="140" zoomScaleNormal="140" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="A31" activeCellId="0" sqref="A31"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultColWidth="11.53515625" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetData/>
+  <printOptions headings="false" gridLines="false" gridLinesSet="true" horizontalCentered="false" verticalCentered="false"/>
+  <pageMargins left="0.7875" right="0.7875" top="1.05277777777778" bottom="1.05277777777778" header="0.7875" footer="0.7875"/>
+  <pageSetup paperSize="1" scale="100" fitToWidth="1" fitToHeight="1" pageOrder="downThenOver" orientation="portrait" blackAndWhite="false" draft="false" cellComments="none" horizontalDpi="300" verticalDpi="300" copies="1"/>
+  <headerFooter differentFirst="false" differentOddEven="false">
+    <oddHeader>&amp;C&amp;"Times New Roman,Regular"&amp;12&amp;Kffffff&amp;A</oddHeader>
+    <oddFooter>&amp;C&amp;"Times New Roman,Regular"&amp;12&amp;KffffffPage &amp;P</oddFooter>
+  </headerFooter>
+  <drawing r:id="rId1"/>
+</worksheet>
 </file>
</xml_diff>